<commit_message>
Evidence for B1 and B2
</commit_message>
<xml_diff>
--- a/gjermundgaraba/evidence.xlsx
+++ b/gjermundgaraba/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t xml:space="preserve">D1BE0624F5A2E777E490AB4A23C179BCCD70F51BDB0143B5E7B85082B96C6736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF1BD8D848698E0191682B54A44E53907F41C0F24C0FDBC633E501BCE76CA950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9B0D38D1734D46EB1BD153ACA28D3AC8E162B4DBC45667E466C31796782E48E2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">773DDA05B751D44A7F0790B9F9C413DEF0B46AFAC7DF04F2E838313D29B09942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1205982C049208BC3E6B91A0D09477ADAE1F79F74E5922524ED57002C3704E78</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -501,10 +513,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -590,7 +602,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -633,7 +645,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -676,7 +688,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -719,7 +731,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -759,10 +771,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
   </cols>
@@ -829,7 +841,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -896,7 +908,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -963,7 +975,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1030,7 +1042,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1097,7 +1109,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1164,7 +1176,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
   </cols>
@@ -1207,7 +1219,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1290,7 +1302,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1370,10 +1382,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1409,10 +1421,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1421,12 +1433,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1447,11 +1459,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1460,12 +1472,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1502,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1499,12 +1511,12 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +1541,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1586,11 +1598,11 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1646,7 +1658,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1702,7 +1714,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
@@ -1758,7 +1770,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
@@ -1816,7 +1828,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>
@@ -1859,7 +1871,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="13.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
   </cols>

</xml_diff>